<commit_message>
change text column: 'theo y/c' ---? 'hỗ trợ'
</commit_message>
<xml_diff>
--- a/banhang24/Template/ImportExcel/FileImport_CaiDatHoaHong.xlsx
+++ b/banhang24/Template/ImportExcel/FileImport_CaiDatHoaHong.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\banhang24_20180625\banhang24vn\banhang24\Template\ImportExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\KangJinDemo\KangJinDemo\banhang24\Template\ImportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,9 +35,6 @@
     <t>Hoa hồng thực hiện</t>
   </si>
   <si>
-    <t>Hoa hồng theo yêu cầu</t>
-  </si>
-  <si>
     <t>Hoa hồng tư vấn</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>HH00113</t>
+  </si>
+  <si>
+    <t>Hoa hồng hỗ trợ</t>
   </si>
 </sst>
 </file>
@@ -225,6 +225,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,7 +241,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,80 +541,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="A1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="J3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="16">
+      <c r="D4" s="11">
         <v>10</v>
       </c>
       <c r="E4" s="6"/>
@@ -632,10 +632,10 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>

</xml_diff>